<commit_message>
icluded no covid test
</commit_message>
<xml_diff>
--- a/ind.xlsx
+++ b/ind.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,7 +455,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>201939</v>
+        <v>201910</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -473,7 +473,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>201940</v>
+        <v>201911</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -491,7 +491,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>201941</v>
+        <v>201912</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -509,7 +509,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>201942</v>
+        <v>201913</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -527,7 +527,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>201943</v>
+        <v>201914</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -545,7 +545,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>201944</v>
+        <v>201915</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -563,7 +563,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>201945</v>
+        <v>201916</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -581,7 +581,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>201946</v>
+        <v>201917</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -599,7 +599,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>201947</v>
+        <v>201918</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -617,7 +617,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>201948</v>
+        <v>201919</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -635,7 +635,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>201949</v>
+        <v>201920</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -653,7 +653,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>201950</v>
+        <v>201921</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -671,7 +671,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>201951</v>
+        <v>201922</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -689,7 +689,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>201952</v>
+        <v>201923</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -707,7 +707,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>202001</v>
+        <v>201924</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -716,7 +716,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2019</t>
         </is>
       </c>
     </row>
@@ -725,7 +725,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>202002</v>
+        <v>201925</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -734,7 +734,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2019</t>
         </is>
       </c>
     </row>
@@ -743,7 +743,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>202003</v>
+        <v>201926</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -752,259 +752,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>202004</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>fast_duck</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>202005</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>fast_duck</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>202006</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>fast_duck</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="n">
-        <v>202007</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>fast_duck</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="n">
-        <v>202008</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>fast_duck</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="n">
-        <v>202009</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>fast_duck</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="n">
-        <v>202010</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>fast_duck</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="n">
-        <v>202011</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>fast_duck</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="n">
-        <v>202012</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>fast_duck</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="n">
-        <v>202013</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>fast_duck</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="n">
-        <v>202014</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>fast_duck</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="n">
-        <v>202015</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>fast_duck</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="n">
-        <v>202016</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>fast_duck</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="n">
-        <v>202017</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>fast_duck</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>2020</t>
+          <t>2019</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
estimator runs but parameters are created for each week
</commit_message>
<xml_diff>
--- a/ind.xlsx
+++ b/ind.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,7 +455,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>201910</v>
+        <v>201827</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -464,7 +464,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -473,7 +473,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>201911</v>
+        <v>201828</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -482,7 +482,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>201912</v>
+        <v>201829</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -500,7 +500,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -509,7 +509,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>201913</v>
+        <v>201830</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -518,7 +518,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>201914</v>
+        <v>201831</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -536,7 +536,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -545,7 +545,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>201915</v>
+        <v>201832</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -554,7 +554,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -563,7 +563,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>201916</v>
+        <v>201833</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -572,7 +572,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>201917</v>
+        <v>201834</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -590,7 +590,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -599,7 +599,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>201918</v>
+        <v>201835</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -608,7 +608,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -617,7 +617,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>201919</v>
+        <v>201836</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -626,7 +626,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -635,7 +635,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>201920</v>
+        <v>201837</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -644,7 +644,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -653,7 +653,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>201921</v>
+        <v>201838</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -662,7 +662,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>201922</v>
+        <v>201839</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -680,7 +680,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -689,7 +689,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>201923</v>
+        <v>201840</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -698,7 +698,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -707,7 +707,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>201924</v>
+        <v>201841</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -716,7 +716,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -725,7 +725,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>201925</v>
+        <v>201842</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -734,7 +734,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -743,16 +743,2536 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
+        <v>201843</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>201844</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>201845</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>201846</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>201847</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>201848</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>201849</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>201850</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>201851</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>201852</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>201901</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>201902</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>201903</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>201904</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>201905</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>201906</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>201907</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>201908</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>201909</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>201910</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>201911</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>201912</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>201913</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>201914</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>201915</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>201916</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>201917</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>201918</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>201919</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>201920</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>201921</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>201922</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>201923</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>201924</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>201925</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
         <v>201926</v>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>fast_duck</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>2019</t>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>201927</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>201928</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>201929</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>201930</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>201931</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>201932</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>201933</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>201934</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>201935</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>201936</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>201937</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>201938</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>201939</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>201940</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>201941</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>201942</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>201943</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>201944</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>201945</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="n">
+        <v>201946</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="n">
+        <v>201947</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="n">
+        <v>201948</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="n">
+        <v>201949</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="n">
+        <v>201950</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="n">
+        <v>201951</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="n">
+        <v>201952</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="n">
+        <v>202001</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="n">
+        <v>202002</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="n">
+        <v>202003</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="n">
+        <v>202004</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="n">
+        <v>202005</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="n">
+        <v>202006</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="n">
+        <v>202007</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="n">
+        <v>202008</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="n">
+        <v>202009</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="n">
+        <v>202010</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="n">
+        <v>202011</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="n">
+        <v>202012</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="n">
+        <v>202013</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="n">
+        <v>202014</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="n">
+        <v>202015</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="n">
+        <v>202016</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="n">
+        <v>202017</v>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="n">
+        <v>202018</v>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="n">
+        <v>202019</v>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="n">
+        <v>202020</v>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="n">
+        <v>202021</v>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="n">
+        <v>202022</v>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="n">
+        <v>202023</v>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="n">
+        <v>202024</v>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="n">
+        <v>202025</v>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="n">
+        <v>202026</v>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="n">
+        <v>202027</v>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="n">
+        <v>202028</v>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="n">
+        <v>202029</v>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="n">
+        <v>202030</v>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="n">
+        <v>202031</v>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="n">
+        <v>202032</v>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="n">
+        <v>202033</v>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="n">
+        <v>202034</v>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" t="n">
+        <v>202035</v>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="n">
+        <v>202036</v>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="n">
+        <v>202037</v>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="n">
+        <v>202038</v>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" t="n">
+        <v>202039</v>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" t="n">
+        <v>202040</v>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" t="n">
+        <v>202041</v>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" t="n">
+        <v>202042</v>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" t="n">
+        <v>202043</v>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" t="n">
+        <v>202044</v>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" t="n">
+        <v>202045</v>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" t="n">
+        <v>202046</v>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" t="n">
+        <v>202047</v>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" t="n">
+        <v>202048</v>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" t="n">
+        <v>202049</v>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" t="n">
+        <v>202050</v>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" t="n">
+        <v>202051</v>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="n">
+        <v>202052</v>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="n">
+        <v>202053</v>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="n">
+        <v>202101</v>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="n">
+        <v>202102</v>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="n">
+        <v>202103</v>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="n">
+        <v>202104</v>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="n">
+        <v>202105</v>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="n">
+        <v>202106</v>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="n">
+        <v>202107</v>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" t="n">
+        <v>202108</v>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="n">
+        <v>202109</v>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="n">
+        <v>202110</v>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" t="n">
+        <v>202111</v>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="n">
+        <v>202112</v>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="n">
+        <v>202113</v>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" t="n">
+        <v>202114</v>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" t="n">
+        <v>202115</v>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" t="n">
+        <v>202116</v>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" t="n">
+        <v>202117</v>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" t="n">
+        <v>202118</v>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B151" t="n">
+        <v>202119</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B152" t="n">
+        <v>202120</v>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B153" t="n">
+        <v>202121</v>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B154" t="n">
+        <v>202122</v>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="B155" t="n">
+        <v>202123</v>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B156" t="n">
+        <v>202124</v>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="B157" t="n">
+        <v>202125</v>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="B158" t="n">
+        <v>202126</v>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>fast_duck</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>2021</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
trained on two, second brand scaled too small
</commit_message>
<xml_diff>
--- a/ind.xlsx
+++ b/ind.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D158"/>
+  <dimension ref="A1:D315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3276,6 +3276,2832 @@
         </is>
       </c>
     </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="B159" t="n">
+        <v>201827</v>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B160" t="n">
+        <v>201828</v>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="B161" t="n">
+        <v>201829</v>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="B162" t="n">
+        <v>201830</v>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B163" t="n">
+        <v>201831</v>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B164" t="n">
+        <v>201832</v>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B165" t="n">
+        <v>201833</v>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="B166" t="n">
+        <v>201834</v>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="B167" t="n">
+        <v>201835</v>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="B168" t="n">
+        <v>201836</v>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="B169" t="n">
+        <v>201837</v>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="B170" t="n">
+        <v>201838</v>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="n">
+        <v>169</v>
+      </c>
+      <c r="B171" t="n">
+        <v>201839</v>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="B172" t="n">
+        <v>201840</v>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="B173" t="n">
+        <v>201841</v>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="B174" t="n">
+        <v>201842</v>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="B175" t="n">
+        <v>201843</v>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="B176" t="n">
+        <v>201844</v>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B177" t="n">
+        <v>201845</v>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="B178" t="n">
+        <v>201846</v>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="B179" t="n">
+        <v>201847</v>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="B180" t="n">
+        <v>201848</v>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="B181" t="n">
+        <v>201849</v>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="B182" t="n">
+        <v>201850</v>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="B183" t="n">
+        <v>201851</v>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="B184" t="n">
+        <v>201852</v>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="n">
+        <v>183</v>
+      </c>
+      <c r="B185" t="n">
+        <v>201901</v>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="n">
+        <v>184</v>
+      </c>
+      <c r="B186" t="n">
+        <v>201902</v>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="B187" t="n">
+        <v>201903</v>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="n">
+        <v>186</v>
+      </c>
+      <c r="B188" t="n">
+        <v>201904</v>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="B189" t="n">
+        <v>201905</v>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="n">
+        <v>188</v>
+      </c>
+      <c r="B190" t="n">
+        <v>201906</v>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="n">
+        <v>189</v>
+      </c>
+      <c r="B191" t="n">
+        <v>201907</v>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="B192" t="n">
+        <v>201908</v>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="n">
+        <v>191</v>
+      </c>
+      <c r="B193" t="n">
+        <v>201909</v>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="B194" t="n">
+        <v>201910</v>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="B195" t="n">
+        <v>201911</v>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="n">
+        <v>194</v>
+      </c>
+      <c r="B196" t="n">
+        <v>201912</v>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="n">
+        <v>195</v>
+      </c>
+      <c r="B197" t="n">
+        <v>201913</v>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="n">
+        <v>196</v>
+      </c>
+      <c r="B198" t="n">
+        <v>201914</v>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="B199" t="n">
+        <v>201915</v>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="B200" t="n">
+        <v>201916</v>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="n">
+        <v>199</v>
+      </c>
+      <c r="B201" t="n">
+        <v>201917</v>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="B202" t="n">
+        <v>201918</v>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B203" t="n">
+        <v>201919</v>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="n">
+        <v>202</v>
+      </c>
+      <c r="B204" t="n">
+        <v>201920</v>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="1" t="n">
+        <v>203</v>
+      </c>
+      <c r="B205" t="n">
+        <v>201921</v>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="1" t="n">
+        <v>204</v>
+      </c>
+      <c r="B206" t="n">
+        <v>201922</v>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="B207" t="n">
+        <v>201923</v>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="B208" t="n">
+        <v>201924</v>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="1" t="n">
+        <v>207</v>
+      </c>
+      <c r="B209" t="n">
+        <v>201925</v>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="B210" t="n">
+        <v>201926</v>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="B211" t="n">
+        <v>201927</v>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="B212" t="n">
+        <v>201928</v>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B213" t="n">
+        <v>201929</v>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="B214" t="n">
+        <v>201930</v>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="n">
+        <v>201931</v>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="n">
+        <v>201932</v>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="n">
+        <v>201933</v>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" t="n">
+        <v>201934</v>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" t="n">
+        <v>201935</v>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="B220" t="n">
+        <v>201936</v>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="B221" t="n">
+        <v>201937</v>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="B222" t="n">
+        <v>201938</v>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="n">
+        <v>221</v>
+      </c>
+      <c r="B223" t="n">
+        <v>201939</v>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>222</v>
+      </c>
+      <c r="B224" t="n">
+        <v>201940</v>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B225" t="n">
+        <v>201941</v>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="B226" t="n">
+        <v>201942</v>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B227" t="n">
+        <v>201943</v>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="n">
+        <v>226</v>
+      </c>
+      <c r="B228" t="n">
+        <v>201944</v>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="n">
+        <v>227</v>
+      </c>
+      <c r="B229" t="n">
+        <v>201945</v>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="B230" t="n">
+        <v>201946</v>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B231" t="n">
+        <v>201947</v>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="1" t="n">
+        <v>230</v>
+      </c>
+      <c r="B232" t="n">
+        <v>201948</v>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="1" t="n">
+        <v>231</v>
+      </c>
+      <c r="B233" t="n">
+        <v>201949</v>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="n">
+        <v>232</v>
+      </c>
+      <c r="B234" t="n">
+        <v>201950</v>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="1" t="n">
+        <v>233</v>
+      </c>
+      <c r="B235" t="n">
+        <v>201951</v>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="n">
+        <v>234</v>
+      </c>
+      <c r="B236" t="n">
+        <v>201952</v>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="n">
+        <v>235</v>
+      </c>
+      <c r="B237" t="n">
+        <v>202001</v>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="1" t="n">
+        <v>236</v>
+      </c>
+      <c r="B238" t="n">
+        <v>202002</v>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="1" t="n">
+        <v>237</v>
+      </c>
+      <c r="B239" t="n">
+        <v>202003</v>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="1" t="n">
+        <v>238</v>
+      </c>
+      <c r="B240" t="n">
+        <v>202004</v>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="1" t="n">
+        <v>239</v>
+      </c>
+      <c r="B241" t="n">
+        <v>202005</v>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="1" t="n">
+        <v>240</v>
+      </c>
+      <c r="B242" t="n">
+        <v>202006</v>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="1" t="n">
+        <v>241</v>
+      </c>
+      <c r="B243" t="n">
+        <v>202007</v>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="1" t="n">
+        <v>242</v>
+      </c>
+      <c r="B244" t="n">
+        <v>202008</v>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="1" t="n">
+        <v>243</v>
+      </c>
+      <c r="B245" t="n">
+        <v>202009</v>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="1" t="n">
+        <v>244</v>
+      </c>
+      <c r="B246" t="n">
+        <v>202010</v>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="1" t="n">
+        <v>245</v>
+      </c>
+      <c r="B247" t="n">
+        <v>202011</v>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="1" t="n">
+        <v>246</v>
+      </c>
+      <c r="B248" t="n">
+        <v>202012</v>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="1" t="n">
+        <v>247</v>
+      </c>
+      <c r="B249" t="n">
+        <v>202013</v>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="1" t="n">
+        <v>248</v>
+      </c>
+      <c r="B250" t="n">
+        <v>202014</v>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="1" t="n">
+        <v>249</v>
+      </c>
+      <c r="B251" t="n">
+        <v>202015</v>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="B252" t="n">
+        <v>202016</v>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="1" t="n">
+        <v>251</v>
+      </c>
+      <c r="B253" t="n">
+        <v>202017</v>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="1" t="n">
+        <v>252</v>
+      </c>
+      <c r="B254" t="n">
+        <v>202018</v>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="1" t="n">
+        <v>253</v>
+      </c>
+      <c r="B255" t="n">
+        <v>202019</v>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="1" t="n">
+        <v>254</v>
+      </c>
+      <c r="B256" t="n">
+        <v>202020</v>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="B257" t="n">
+        <v>202021</v>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="1" t="n">
+        <v>256</v>
+      </c>
+      <c r="B258" t="n">
+        <v>202022</v>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="1" t="n">
+        <v>257</v>
+      </c>
+      <c r="B259" t="n">
+        <v>202023</v>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="1" t="n">
+        <v>258</v>
+      </c>
+      <c r="B260" t="n">
+        <v>202024</v>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="1" t="n">
+        <v>259</v>
+      </c>
+      <c r="B261" t="n">
+        <v>202025</v>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="1" t="n">
+        <v>260</v>
+      </c>
+      <c r="B262" t="n">
+        <v>202026</v>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="1" t="n">
+        <v>261</v>
+      </c>
+      <c r="B263" t="n">
+        <v>202027</v>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="1" t="n">
+        <v>262</v>
+      </c>
+      <c r="B264" t="n">
+        <v>202028</v>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="1" t="n">
+        <v>263</v>
+      </c>
+      <c r="B265" t="n">
+        <v>202029</v>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="1" t="n">
+        <v>264</v>
+      </c>
+      <c r="B266" t="n">
+        <v>202030</v>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="B267" t="n">
+        <v>202031</v>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="1" t="n">
+        <v>266</v>
+      </c>
+      <c r="B268" t="n">
+        <v>202032</v>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="B269" t="n">
+        <v>202033</v>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="1" t="n">
+        <v>268</v>
+      </c>
+      <c r="B270" t="n">
+        <v>202034</v>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="1" t="n">
+        <v>269</v>
+      </c>
+      <c r="B271" t="n">
+        <v>202035</v>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="1" t="n">
+        <v>270</v>
+      </c>
+      <c r="B272" t="n">
+        <v>202036</v>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="1" t="n">
+        <v>271</v>
+      </c>
+      <c r="B273" t="n">
+        <v>202037</v>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="1" t="n">
+        <v>272</v>
+      </c>
+      <c r="B274" t="n">
+        <v>202038</v>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="1" t="n">
+        <v>273</v>
+      </c>
+      <c r="B275" t="n">
+        <v>202039</v>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="1" t="n">
+        <v>274</v>
+      </c>
+      <c r="B276" t="n">
+        <v>202040</v>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="1" t="n">
+        <v>275</v>
+      </c>
+      <c r="B277" t="n">
+        <v>202041</v>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="1" t="n">
+        <v>276</v>
+      </c>
+      <c r="B278" t="n">
+        <v>202042</v>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="1" t="n">
+        <v>277</v>
+      </c>
+      <c r="B279" t="n">
+        <v>202043</v>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="1" t="n">
+        <v>278</v>
+      </c>
+      <c r="B280" t="n">
+        <v>202044</v>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="1" t="n">
+        <v>279</v>
+      </c>
+      <c r="B281" t="n">
+        <v>202045</v>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="1" t="n">
+        <v>280</v>
+      </c>
+      <c r="B282" t="n">
+        <v>202046</v>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="1" t="n">
+        <v>281</v>
+      </c>
+      <c r="B283" t="n">
+        <v>202047</v>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="1" t="n">
+        <v>282</v>
+      </c>
+      <c r="B284" t="n">
+        <v>202048</v>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="1" t="n">
+        <v>283</v>
+      </c>
+      <c r="B285" t="n">
+        <v>202049</v>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="1" t="n">
+        <v>284</v>
+      </c>
+      <c r="B286" t="n">
+        <v>202050</v>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="1" t="n">
+        <v>285</v>
+      </c>
+      <c r="B287" t="n">
+        <v>202051</v>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="1" t="n">
+        <v>286</v>
+      </c>
+      <c r="B288" t="n">
+        <v>202052</v>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="1" t="n">
+        <v>287</v>
+      </c>
+      <c r="B289" t="n">
+        <v>202053</v>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="1" t="n">
+        <v>288</v>
+      </c>
+      <c r="B290" t="n">
+        <v>202101</v>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="1" t="n">
+        <v>289</v>
+      </c>
+      <c r="B291" t="n">
+        <v>202102</v>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="1" t="n">
+        <v>290</v>
+      </c>
+      <c r="B292" t="n">
+        <v>202103</v>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="1" t="n">
+        <v>291</v>
+      </c>
+      <c r="B293" t="n">
+        <v>202104</v>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="1" t="n">
+        <v>292</v>
+      </c>
+      <c r="B294" t="n">
+        <v>202105</v>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="1" t="n">
+        <v>293</v>
+      </c>
+      <c r="B295" t="n">
+        <v>202106</v>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="1" t="n">
+        <v>294</v>
+      </c>
+      <c r="B296" t="n">
+        <v>202107</v>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="1" t="n">
+        <v>295</v>
+      </c>
+      <c r="B297" t="n">
+        <v>202108</v>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="1" t="n">
+        <v>296</v>
+      </c>
+      <c r="B298" t="n">
+        <v>202109</v>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="1" t="n">
+        <v>297</v>
+      </c>
+      <c r="B299" t="n">
+        <v>202110</v>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="1" t="n">
+        <v>298</v>
+      </c>
+      <c r="B300" t="n">
+        <v>202111</v>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="1" t="n">
+        <v>299</v>
+      </c>
+      <c r="B301" t="n">
+        <v>202112</v>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="B302" t="n">
+        <v>202113</v>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="1" t="n">
+        <v>301</v>
+      </c>
+      <c r="B303" t="n">
+        <v>202114</v>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="1" t="n">
+        <v>302</v>
+      </c>
+      <c r="B304" t="n">
+        <v>202115</v>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="1" t="n">
+        <v>303</v>
+      </c>
+      <c r="B305" t="n">
+        <v>202116</v>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" s="1" t="n">
+        <v>304</v>
+      </c>
+      <c r="B306" t="n">
+        <v>202117</v>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="1" t="n">
+        <v>305</v>
+      </c>
+      <c r="B307" t="n">
+        <v>202118</v>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="1" t="n">
+        <v>306</v>
+      </c>
+      <c r="B308" t="n">
+        <v>202119</v>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" s="1" t="n">
+        <v>307</v>
+      </c>
+      <c r="B309" t="n">
+        <v>202120</v>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="1" t="n">
+        <v>308</v>
+      </c>
+      <c r="B310" t="n">
+        <v>202121</v>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="1" t="n">
+        <v>309</v>
+      </c>
+      <c r="B311" t="n">
+        <v>202122</v>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" s="1" t="n">
+        <v>310</v>
+      </c>
+      <c r="B312" t="n">
+        <v>202123</v>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="1" t="n">
+        <v>311</v>
+      </c>
+      <c r="B313" t="n">
+        <v>202124</v>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="1" t="n">
+        <v>312</v>
+      </c>
+      <c r="B314" t="n">
+        <v>202125</v>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="1" t="n">
+        <v>313</v>
+      </c>
+      <c r="B315" t="n">
+        <v>202126</v>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>gold_plane</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>